<commit_message>
Added info to Use Case Scenarios, Product Backlog, Sprint Backlog
</commit_message>
<xml_diff>
--- a/sprints/sprint1/Sprint 1 Backlog Burndown Chart.xlsx
+++ b/sprints/sprint1/Sprint 1 Backlog Burndown Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wtjra\OneDrive\Desktop\SeProject\UWG-SE2-Spring22-Team4\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\CS Courses\CS3212\SE2 Project\UWG-SE2-Spring22-Team4\sprints\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61791041-5DBB-4410-AEE0-261AC61CBA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DBA407-9CC2-4B7F-BF4A-F0A6D4A8B24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Related User Story</t>
   </si>
@@ -107,9 +109,6 @@
     <t>Preferences class - list of selected days and muscle groups</t>
   </si>
   <si>
-    <t>I/O interface - load() and save()</t>
-  </si>
-  <si>
     <t>Calendar data binding</t>
   </si>
   <si>
@@ -125,9 +124,6 @@
     <t>Create User class - Preferences, Calendar, Login credentials</t>
   </si>
   <si>
-    <t>Dummy loader class - FileWriter, FileReader</t>
-  </si>
-  <si>
     <t>WorkoutGenerator class - API query handler, "intelligent" workout programming</t>
   </si>
   <si>
@@ -144,6 +140,12 @@
   </si>
   <si>
     <t>Jordan</t>
+  </si>
+  <si>
+    <t>User Data I/O</t>
+  </si>
+  <si>
+    <t>Tyler (PP)</t>
   </si>
 </sst>
 </file>
@@ -341,20 +343,23 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$32:$H$32</c:f>
+              <c:f>Sheet1!$D$31:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1105,7 +1110,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1397,21 +1402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1"/>
-    <col min="2" max="2" width="67.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.453125" customWidth="1"/>
+    <col min="2" max="2" width="67.36328125" customWidth="1"/>
+    <col min="3" max="3" width="34.08984375" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -1431,7 +1436,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1449,15 +1454,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1471,15 +1476,17 @@
       <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -1493,15 +1500,17 @@
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1515,15 +1524,17 @@
       <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1537,47 +1548,65 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1591,216 +1620,262 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
       <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>34</v>
@@ -1808,30 +1883,30 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
       <c r="G20" s="2">
         <v>1</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1841,7 +1916,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1851,7 +1926,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1861,7 +1936,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1871,7 +1946,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1881,7 +1956,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1891,7 +1966,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1901,7 +1976,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1911,7 +1986,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1921,39 +1996,29 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3">
-        <f>SUM(D3:D31)</f>
-        <v>22</v>
-      </c>
-      <c r="E32" s="3">
-        <f>SUM(E3:E31)</f>
-        <v>10</v>
-      </c>
-      <c r="F32" s="3">
-        <f>SUM(F3:F31)</f>
-        <v>9</v>
-      </c>
-      <c r="G32" s="3">
-        <f>SUM(G3:G31)</f>
-        <v>7</v>
-      </c>
-      <c r="H32" s="3">
-        <f>SUM(H3:H31)</f>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3">
+        <f>SUM(D3:D30)</f>
+        <v>20</v>
+      </c>
+      <c r="E31" s="3">
+        <f>SUM(E3:E30)</f>
+        <v>17</v>
+      </c>
+      <c r="F31" s="3">
+        <f>SUM(F3:F30)</f>
+        <v>14</v>
+      </c>
+      <c r="G31" s="3">
+        <f>SUM(G3:G30)</f>
+        <v>5</v>
+      </c>
+      <c r="H31" s="3">
+        <f>SUM(H3:H30)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>